<commit_message>
all guild inventory update
</commit_message>
<xml_diff>
--- a/Void/inventory.xlsx
+++ b/Void/inventory.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
   <si>
     <t>Barracus</t>
   </si>
@@ -35,9 +35,6 @@
     <t xml:space="preserve"> Alaric</t>
   </si>
   <si>
-    <t xml:space="preserve"> Xillanail</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Auger Ream</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t xml:space="preserve"> Elite Squadron</t>
   </si>
   <si>
-    <t>Kylen</t>
-  </si>
-  <si>
     <t>Deranged Fanatic</t>
   </si>
   <si>
@@ -116,24 +110,9 @@
     <t>nexor</t>
   </si>
   <si>
-    <t xml:space="preserve"> tremor wyrm</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Tartarus Brood</t>
   </si>
   <si>
-    <t>baughe x2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> elite soldier</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> xeno overlord</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> masterwork aegis</t>
-  </si>
-  <si>
     <t>Xeno Suzerain</t>
   </si>
   <si>
@@ -176,36 +155,12 @@
     <t xml:space="preserve"> Nesxusis</t>
   </si>
   <si>
-    <t>Auger (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Xeno Suzerian</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Onyx (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Marshall (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ezimit(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dreamweaver (3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quake (4)</t>
-  </si>
-  <si>
     <t>Spitful Raptor</t>
   </si>
   <si>
     <t xml:space="preserve"> Radar Sentry</t>
   </si>
   <si>
-    <t>Inferno Demon (2). Shock Disruptor (2)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Warhead</t>
   </si>
   <si>
@@ -288,6 +243,27 @@
   </si>
   <si>
     <t>Bane of Truth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Baughe</t>
+  </si>
+  <si>
+    <t>Draconian Sovereign</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Toxic Tank</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Necropocalypse</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Howling Malgoth</t>
+  </si>
+  <si>
+    <t>Inferno Demon (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shock Disruptor (2)</t>
   </si>
 </sst>
 </file>
@@ -647,27 +623,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A45"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="22.28515625" style="1"/>
+    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="22.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -675,401 +654,399 @@
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1" t="s">
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:10" ht="78" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="78" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="D31" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="E31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="78" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>68</v>
-      </c>
+    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-    </row>
-    <row r="36" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H36" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2"/>
-    </row>
-    <row r="44" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A43" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2"/>
     </row>
     <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2"/>
+      <c r="A45" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2"/>
+    </row>
+    <row r="49" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2"/>
+    </row>
+    <row r="50" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A2:C51">

</xml_diff>